<commit_message>
Actualizat fisa 3 excel
</commit_message>
<xml_diff>
--- a/excel/fisa_excel_functii.xlsx
+++ b/excel/fisa_excel_functii.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
   <si>
     <t>Cod_elev</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>Media anuala 2022</t>
+  </si>
+  <si>
+    <t>Sortati datele descrescator in functie de media anuala</t>
   </si>
 </sst>
 </file>
@@ -372,9 +375,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -408,8 +411,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,6 +448,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,13 +486,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -479,6 +502,9 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -784,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G17" sqref="G17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -868,7 +894,7 @@
         <v>9.18</v>
       </c>
       <c r="E4" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>103</v>
@@ -889,7 +915,7 @@
         <v>8.83</v>
       </c>
       <c r="E5" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -906,7 +932,7 @@
         <v>9.0299999999999994</v>
       </c>
       <c r="E6" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>104</v>
@@ -927,7 +953,7 @@
         <v>8.5</v>
       </c>
       <c r="E7" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>105</v>
@@ -948,7 +974,7 @@
         <v>7.2</v>
       </c>
       <c r="E8" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -969,7 +995,7 @@
         <v>8.84</v>
       </c>
       <c r="E9" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>106</v>
@@ -990,7 +1016,7 @@
         <v>8.9</v>
       </c>
       <c r="E10" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>107</v>
@@ -1011,7 +1037,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E11" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>108</v>
@@ -1032,14 +1058,14 @@
         <v>8.5299999999999994</v>
       </c>
       <c r="E12" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>109</v>
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10007</v>
       </c>
@@ -1053,9 +1079,9 @@
         <v>8.93</v>
       </c>
       <c r="E13" s="3">
-        <v>1500000</v>
-      </c>
-      <c r="G13" s="8" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>110</v>
       </c>
       <c r="H13" s="7"/>
@@ -1074,7 +1100,7 @@
         <v>8.9600000000000009</v>
       </c>
       <c r="E14" s="3">
-        <v>1500000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1091,7 +1117,7 @@
         <v>8.7100000000000009</v>
       </c>
       <c r="E15" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>111</v>
@@ -1112,10 +1138,10 @@
         <v>7.86</v>
       </c>
       <c r="E16" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>10088</v>
       </c>
@@ -1129,10 +1155,15 @@
         <v>7.36</v>
       </c>
       <c r="E17" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>10014</v>
       </c>
@@ -1146,10 +1177,10 @@
         <v>8.68</v>
       </c>
       <c r="E18" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>10021</v>
       </c>
@@ -1163,10 +1194,10 @@
         <v>7.93</v>
       </c>
       <c r="E19" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>10045</v>
       </c>
@@ -1180,10 +1211,10 @@
         <v>7</v>
       </c>
       <c r="E20" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>10070</v>
       </c>
@@ -1197,10 +1228,10 @@
         <v>8.23</v>
       </c>
       <c r="E21" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>10016</v>
       </c>
@@ -1214,10 +1245,10 @@
         <v>8.56</v>
       </c>
       <c r="E22" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>10083</v>
       </c>
@@ -1231,10 +1262,10 @@
         <v>8.1</v>
       </c>
       <c r="E23" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>10073</v>
       </c>
@@ -1248,10 +1279,10 @@
         <v>9.5</v>
       </c>
       <c r="E24" s="3">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>10027</v>
       </c>
@@ -1265,10 +1296,10 @@
         <v>8.59</v>
       </c>
       <c r="E25" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>10056</v>
       </c>
@@ -1282,10 +1313,10 @@
         <v>8.85</v>
       </c>
       <c r="E26" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>10086</v>
       </c>
@@ -1299,10 +1330,10 @@
         <v>7.93</v>
       </c>
       <c r="E27" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>10009</v>
       </c>
@@ -1316,10 +1347,10 @@
         <v>8.84</v>
       </c>
       <c r="E28" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>10019</v>
       </c>
@@ -1333,10 +1364,10 @@
         <v>8.36</v>
       </c>
       <c r="E29" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>10040</v>
       </c>
@@ -1350,10 +1381,10 @@
         <v>8.18</v>
       </c>
       <c r="E30" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>10037</v>
       </c>
@@ -1367,10 +1398,10 @@
         <v>8.25</v>
       </c>
       <c r="E31" s="3">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>10035</v>
       </c>
@@ -1384,7 +1415,7 @@
         <v>8.34</v>
       </c>
       <c r="E32" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1401,7 +1432,7 @@
         <v>8.73</v>
       </c>
       <c r="E33" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1418,7 +1449,7 @@
         <v>8.1300000000000008</v>
       </c>
       <c r="E34" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1435,7 +1466,7 @@
         <v>8.33</v>
       </c>
       <c r="E35" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1467,7 +1498,7 @@
         <v>9.31</v>
       </c>
       <c r="E37" s="3">
-        <v>2500000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1484,7 +1515,7 @@
         <v>8.23</v>
       </c>
       <c r="E38" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1501,7 +1532,7 @@
         <v>9.26</v>
       </c>
       <c r="E39" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1518,7 +1549,7 @@
         <v>8.4</v>
       </c>
       <c r="E40" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1535,7 +1566,7 @@
         <v>8.76</v>
       </c>
       <c r="E41" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1552,7 +1583,7 @@
         <v>8.86</v>
       </c>
       <c r="E42" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1569,7 +1600,7 @@
         <v>8.2100000000000009</v>
       </c>
       <c r="E43" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1586,7 +1617,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="E44" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1603,7 +1634,7 @@
         <v>8.5</v>
       </c>
       <c r="E45" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1620,7 +1651,7 @@
         <v>8.4</v>
       </c>
       <c r="E46" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1637,7 +1668,7 @@
         <v>7.71</v>
       </c>
       <c r="E47" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1654,7 +1685,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E48" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1671,7 +1702,7 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="E49" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1688,7 +1719,7 @@
         <v>8.5</v>
       </c>
       <c r="E50" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1705,7 +1736,7 @@
         <v>7.2</v>
       </c>
       <c r="E51" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1722,7 +1753,7 @@
         <v>8.76</v>
       </c>
       <c r="E52" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1739,7 +1770,7 @@
         <v>9.09</v>
       </c>
       <c r="E53" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1756,7 +1787,7 @@
         <v>8.65</v>
       </c>
       <c r="E54" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1773,7 +1804,7 @@
         <v>8.39</v>
       </c>
       <c r="E55" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1790,7 +1821,7 @@
         <v>8.5299999999999994</v>
       </c>
       <c r="E56" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1807,7 +1838,7 @@
         <v>7.96</v>
       </c>
       <c r="E57" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -1824,7 +1855,7 @@
         <v>9.23</v>
       </c>
       <c r="E58" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1841,7 +1872,7 @@
         <v>7.56</v>
       </c>
       <c r="E59" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1858,7 +1889,7 @@
         <v>8.9</v>
       </c>
       <c r="E60" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1875,7 +1906,7 @@
         <v>8.36</v>
       </c>
       <c r="E61" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1892,7 +1923,7 @@
         <v>9.6</v>
       </c>
       <c r="E62" s="3">
-        <v>2500000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1924,7 +1955,7 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="E64" s="3">
-        <v>2500000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -1941,7 +1972,7 @@
         <v>8.75</v>
       </c>
       <c r="E65" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -1958,7 +1989,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="E66" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -1975,7 +2006,7 @@
         <v>9.6199999999999992</v>
       </c>
       <c r="E67" s="3">
-        <v>2500000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -1992,7 +2023,7 @@
         <v>8.3699999999999992</v>
       </c>
       <c r="E68" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2009,7 +2040,7 @@
         <v>7.71</v>
       </c>
       <c r="E69" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2026,7 +2057,7 @@
         <v>8.1</v>
       </c>
       <c r="E70" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2058,7 +2089,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E72" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2075,7 +2106,7 @@
         <v>8.56</v>
       </c>
       <c r="E73" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2092,7 +2123,7 @@
         <v>8.25</v>
       </c>
       <c r="E74" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2109,7 +2140,7 @@
         <v>8.3699999999999992</v>
       </c>
       <c r="E75" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2126,7 +2157,7 @@
         <v>8.65</v>
       </c>
       <c r="E76" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2143,7 +2174,7 @@
         <v>9</v>
       </c>
       <c r="E77" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2160,7 +2191,7 @@
         <v>8.5</v>
       </c>
       <c r="E78" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2177,7 +2208,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2194,7 +2225,7 @@
         <v>8.76</v>
       </c>
       <c r="E80" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2211,7 +2242,7 @@
         <v>7.33</v>
       </c>
       <c r="E81" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2228,7 +2259,7 @@
         <v>8.93</v>
       </c>
       <c r="E82" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2245,7 +2276,7 @@
         <v>8.9</v>
       </c>
       <c r="E83" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2262,7 +2293,7 @@
         <v>7.63</v>
       </c>
       <c r="E84" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2279,7 +2310,7 @@
         <v>8.59</v>
       </c>
       <c r="E85" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2296,7 +2327,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E86" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2313,7 +2344,7 @@
         <v>8.43</v>
       </c>
       <c r="E87" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2330,7 +2361,7 @@
         <v>8.43</v>
       </c>
       <c r="E88" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2347,7 +2378,7 @@
         <v>8.75</v>
       </c>
       <c r="E89" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2364,7 +2395,7 @@
         <v>7.26</v>
       </c>
       <c r="E90" s="3">
-        <v>500000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -2381,7 +2412,7 @@
         <v>8.2799999999999994</v>
       </c>
       <c r="E91" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2398,7 +2429,7 @@
         <v>8.31</v>
       </c>
       <c r="E92" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2415,7 +2446,7 @@
         <v>9.36</v>
       </c>
       <c r="E93" s="3">
-        <v>2500000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2432,7 +2463,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E94" s="3">
-        <v>2000000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2449,7 +2480,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="E95" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2466,13 +2497,16 @@
         <v>8.33</v>
       </c>
       <c r="E96" s="3">
-        <v>1500000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="102" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E102" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G17:I17"/>
+  </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>